<commit_message>
Add mean and SD table
</commit_message>
<xml_diff>
--- a/results/LIC/LIC_values.xlsx
+++ b/results/LIC/LIC_values.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\ORnearshore_groundfish\results\LIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0C70D7-33C5-4606-8A4B-C5A1C8AC1505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389F67F7-A95A-43CA-BEEF-A2AE6B6DE9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overall LIC" sheetId="1" r:id="rId1"/>
+    <sheet name="Spatially Explicit LIC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Species</t>
   </si>
@@ -58,6 +59,78 @@
   </si>
   <si>
     <t>Dover sole</t>
+  </si>
+  <si>
+    <t>0.0058 ± 0.020</t>
+  </si>
+  <si>
+    <t>0.0013 ± 0.011</t>
+  </si>
+  <si>
+    <t>0.0002 ± 0.001</t>
+  </si>
+  <si>
+    <t>0.0006 ± 0.004</t>
+  </si>
+  <si>
+    <t>0.00005 ± 0.001</t>
+  </si>
+  <si>
+    <t>0.0009 ± 0.006</t>
+  </si>
+  <si>
+    <t>0.0009 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.0033 ± 0.006</t>
+  </si>
+  <si>
+    <t>0.0057 ± 0.008</t>
+  </si>
+  <si>
+    <t>0.0049 ± 0.006</t>
+  </si>
+  <si>
+    <t>0.0012 ± 0.007</t>
+  </si>
+  <si>
+    <t>0.0022 ± 0.013</t>
+  </si>
+  <si>
+    <t>0.0001 ± 0.001</t>
+  </si>
+  <si>
+    <t>0.0025 ± 0.006</t>
+  </si>
+  <si>
+    <t>0.0020 ± 0.004</t>
+  </si>
+  <si>
+    <t>0.0038 ± 0.007</t>
+  </si>
+  <si>
+    <t>0.0032 ± 0.013</t>
+  </si>
+  <si>
+    <t>0.0036 ± 0.024</t>
+  </si>
+  <si>
+    <t>0.0042 ± 0.017</t>
+  </si>
+  <si>
+    <t>0.0038 ± 0.013</t>
+  </si>
+  <si>
+    <t>0.0046 ± 0.010</t>
+  </si>
+  <si>
+    <t>0.0054 ± 0.012</t>
+  </si>
+  <si>
+    <t>0.0059 ± 0.011</t>
+  </si>
+  <si>
+    <t>0.0046 ± 0.008</t>
   </si>
 </sst>
 </file>
@@ -399,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="H1:L7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,4 +706,146 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9287A63B-7394-4F13-9D66-08FE728A73A1}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>